<commit_message>
changed character height to 115
</commit_message>
<xml_diff>
--- a/character_details.xlsx
+++ b/character_details.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>Characters</t>
   </si>
@@ -136,6 +136,21 @@
   </si>
   <si>
     <t>50*115</t>
+  </si>
+  <si>
+    <t>Death</t>
+  </si>
+  <si>
+    <t>Jump</t>
+  </si>
+  <si>
+    <t>Kick</t>
+  </si>
+  <si>
+    <t>Punch</t>
+  </si>
+  <si>
+    <t>Jump Attack</t>
   </si>
 </sst>
 </file>
@@ -452,7 +467,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -460,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -633,6 +648,31 @@
         <v>7</v>
       </c>
     </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>